<commit_message>
updating presentation and plots
</commit_message>
<xml_diff>
--- a/FBProphet/Business Analysis.xlsx
+++ b/FBProphet/Business Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esdras/Ironhack/Proyect/Prophet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esdras/Ironhack/Proyect/FBProphet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8F9B07-AE40-4F4D-8421-8BD83C33E4AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAF0876-F90B-4340-8D01-F3261B94B594}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="27560" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="27560" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="1" r:id="rId1"/>
@@ -669,9 +669,6 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -680,6 +677,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1351,13 +1351,13 @@
       <c r="O8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="18">
         <v>11363</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="Q8" s="18">
         <v>9090</v>
       </c>
-      <c r="R8" s="19">
+      <c r="R8" s="18">
         <v>7727</v>
       </c>
     </row>
@@ -1849,13 +1849,13 @@
       <c r="O18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P18" s="20">
+      <c r="P18" s="19">
         <v>11363</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="19">
         <v>9090</v>
       </c>
-      <c r="R18" s="20">
+      <c r="R18" s="19">
         <v>7727</v>
       </c>
     </row>
@@ -1948,7 +1948,7 @@
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M20" s="20">
         <v>7</v>
       </c>
       <c r="N20" t="s">
@@ -2116,7 +2116,7 @@
         <f t="shared" si="3"/>
         <v>-0.1029284269338214</v>
       </c>
-      <c r="M23" s="21">
+      <c r="M23" s="20">
         <v>2.5</v>
       </c>
       <c r="N23" t="s">
@@ -2279,10 +2279,10 @@
         <f t="shared" si="3"/>
         <v>-0.25376798075506896</v>
       </c>
-      <c r="Q27" s="18" t="s">
+      <c r="Q27" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="R27" s="18"/>
+      <c r="R27" s="21"/>
       <c r="S27" s="14">
         <f>S14-S24</f>
         <v>22953.5</v>
@@ -2303,10 +2303,10 @@
         <f>SUM(G2:G27)</f>
         <v>3606000</v>
       </c>
-      <c r="Q28" s="18" t="s">
+      <c r="Q28" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="R28" s="18"/>
+      <c r="R28" s="21"/>
       <c r="S28" s="14">
         <f>S27*3</f>
         <v>68860.5</v>
@@ -2316,10 +2316,10 @@
       <c r="E29" s="2"/>
       <c r="H29" s="2"/>
       <c r="J29" s="3"/>
-      <c r="Q29" s="18" t="s">
+      <c r="Q29" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="R29" s="18"/>
+      <c r="R29" s="21"/>
       <c r="S29" s="14">
         <f>S28*12</f>
         <v>826326</v>

</xml_diff>